<commit_message>
change led from white to green
</commit_message>
<xml_diff>
--- a/PCB_ROHM_BaAnh/BaAnh_rohm_bom.xlsx
+++ b/PCB_ROHM_BaAnh/BaAnh_rohm_bom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Duy\PCB_ROHM_BaAnh\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C4007FB-D0CD-4697-90A4-4BC91FFF8119}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED6E5D91-593A-4B6C-A7D4-7940B1FAD6BE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="12225" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -68,7 +68,6 @@
         <sz val="11"/>
         <color rgb="FFAFABAB"/>
         <rFont val="宋体"/>
-        <charset val="134"/>
       </rPr>
       <t>（</t>
     </r>
@@ -86,7 +85,6 @@
         <sz val="11"/>
         <color rgb="FFAFABAB"/>
         <rFont val="宋体"/>
-        <charset val="134"/>
       </rPr>
       <t>）</t>
     </r>
@@ -96,9 +94,6 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>C2290</t>
-  </si>
-  <si>
     <t>LED</t>
     <phoneticPr fontId="3"/>
   </si>
@@ -219,13 +214,16 @@
   </si>
   <si>
     <t>TSSOP-20_4.4x6.5x0.65P</t>
+  </si>
+  <si>
+    <t>C165984</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -236,7 +234,6 @@
       <sz val="11"/>
       <color rgb="FFAFABAB"/>
       <name val="宋体"/>
-      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
@@ -281,6 +278,12 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="PingFangSC, PingFangSC-Semibold"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -319,7 +322,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -375,6 +378,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -762,7 +768,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15"/>
@@ -792,7 +798,7 @@
     </row>
     <row r="2" spans="1:5" ht="64.5" customHeight="1">
       <c r="A2" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>12</v>
@@ -800,8 +806,8 @@
       <c r="C2" s="11">
         <v>805</v>
       </c>
-      <c r="D2" s="12" t="s">
-        <v>13</v>
+      <c r="D2" s="19" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1">
@@ -809,41 +815,41 @@
         <v>5</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" s="13">
         <v>805</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1">
       <c r="A4" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" s="13">
         <v>805</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="31.5">
       <c r="A5" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" s="13">
         <v>805</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="78.75">
@@ -851,83 +857,83 @@
         <v>6</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C6" s="13">
         <v>805</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75">
       <c r="A7" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7" s="13">
         <v>805</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75">
       <c r="A8" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C8" s="13">
         <v>805</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75">
       <c r="A9" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="12" t="s">
         <v>32</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75">
       <c r="A10" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C10" s="13">
         <v>805</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="47.25">
       <c r="A11" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C11" s="13">
         <v>805</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75">
@@ -935,27 +941,27 @@
         <v>7</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C12" s="13">
         <v>805</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.75">
       <c r="A13" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C13" s="13">
         <v>805</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="47.25">
@@ -963,10 +969,10 @@
         <v>4</v>
       </c>
       <c r="B14" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="12" t="s">
         <v>45</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>46</v>
       </c>
       <c r="D14" s="12" t="s">
         <v>3</v>
@@ -974,10 +980,10 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C15" s="12" t="s">
         <v>9</v>
@@ -988,13 +994,13 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="12" t="s">
         <v>50</v>
-      </c>
-      <c r="B16" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>51</v>
       </c>
       <c r="D16" s="12" t="s">
         <v>10</v>

</xml_diff>